<commit_message>
merged createHouse and EditHouse components. followed other logic feedbacks
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT-Assessment-Hour-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kantatanahashi/Documents/dtt/dtt-assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDCDEC08-B64D-DA4F-8282-6205AF43CAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327A1BFB-0E14-0C45-84DA-B238E449C190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Subject</t>
   </si>
@@ -315,6 +315,35 @@
   <si>
     <t xml:space="preserve">The user input submitted through the form now goes through validation. Firstly, the system checks whether all the required fiels are filled. Following this, the system ensures the integrity of the inputs by verifying if the inputs are valid. For example, it checks whether numeric inputs, like the price, can be parsed as numbers without problem. If the form validation fails, users will be notified with an error message below the failed input and the border of the input field will become red. 
 Additionally, number inputs are parsed as numbers using parseInt() before POST request is sent to the House API. This adds some flexibility to the user's input. For example, if the user decides to type 60m2 for size instead of just 60, doing parseInt() makes sure that I only take the 60 part and not the unit. </t>
+  </si>
+  <si>
+    <t>General feedback applied</t>
+  </si>
+  <si>
+    <t>Styles/formatting/structure feedback incorporated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The currency formatting has been applied to the prices. There is a filter function created in main.js, which is used in both HouseInfo and HouseDetail components. 
+Max width of the content has been decreased for a larger screen. 
+The action icons of the house detail and the house overview page are now placed in column instead of row. However, for the action icons displayed inside of HousePreview, it was made such that when the width of the screen is very small, they will be placed in row to fit more content within the given width. 
+Styles from the form have been improved, following the style specification given to us. This included the change of font-family for input labels and textarea placeholder and making the input fields border more curvy. 
+Indentation level was made consistent to 2 spaces indentation. 
+The use of axios.defaults.headers.common allowed for setting the request headers for all of the API requests, eliminating the duplicated API keys that I had in my previous impleentation. Furthermore, baseURL and API key has been stored in .env file and is accessed via import.meta.env. 
+&lt;nav&gt; has been used for containing navigation bar content, and &lt;article&gt; has been used to contain a self-contained elements. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Migrated from Vue CLI to Vite. This was done following the tutorial (https://vueschool.io/articles/vuejs-tutorials/how-to-migrate-from-vue-cli-to-vite/)
+&lt;script setup&gt; tag is used as opposed to &lt;script&gt; tag, which allowed me to write a much clearner code. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logic feedback applied </t>
+  </si>
+  <si>
+    <t>CreateHouse and EditHouse components have been deleted and merged into HouseForm component as my previous implementation had many code duplications in the two components. Type of the form (create or edit) has been passed as a route parameter and this is used with v-if: to display the desired title text and corresponding submit buttons (POST or SAVE button) etc
+API to get one house by ID is now used to incorporate users who might open the website from the house detail page. (e.g. http://localhost:8080/houses/2)
+There is no longer a watcher on house detail page that reloads the entire page. Rather, clicking on  recommendation items result in updating the house variable used inside of the template to render the content. Together, recommendation list is updated. To rerender HouseInfo component which is used to display recommendation house information, :key has been used and has been set to equal to recommendation house id. This means that everytime there is an update in the recommendation list, the component gets rerendered to display the latest picked house information. 
+Updating a house results in the user being navigated to the house details page. 
+The use of global CSS is minimized.</t>
   </si>
 </sst>
 </file>
@@ -631,7 +660,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -650,18 +679,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -713,9 +730,6 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -736,6 +750,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1996,8 +2022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2011,380 +2037,404 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="A1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
       <c r="E1" s="9"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="41"/>
     </row>
     <row r="3" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="25" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="258" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="21">
         <v>2</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="22">
         <v>45264</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="91" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="15">
         <v>3</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="16">
         <v>45264</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="17"/>
+      <c r="E5" s="13"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="21">
         <v>2</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="22">
         <v>45264</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="26" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="178" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="21">
         <v>4</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="22">
         <v>45265</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="30"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="101" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="21">
         <v>2</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="22">
         <v>45267</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="30"/>
+      <c r="E8" s="26"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="76" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="15">
         <v>2</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="16">
         <v>45267</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="121" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="15">
         <v>3</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="16">
         <v>45268</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="18"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="141" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="15">
         <v>4</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="16">
         <v>45268</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="17"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="74" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="21">
         <v>2</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="22">
         <v>45269</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="153" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="21">
         <v>3</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="22">
         <v>45270</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="26" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="27">
         <v>1</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="16">
         <v>45271</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="17"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="107" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="21">
         <v>3</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="22">
         <v>45271</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="30"/>
+      <c r="E15" s="26"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="21">
         <v>1</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="22">
         <v>45279</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="26" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="21">
         <v>2</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="22">
         <v>45279</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="30"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="40">
+      <c r="B18" s="35">
         <v>1</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="36">
         <v>45280</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="16"/>
+      <c r="E18" s="12"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="21">
         <v>0</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="22">
         <v>45280</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="30"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="30"/>
+    <row r="20" spans="1:6" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="21">
+        <v>1</v>
+      </c>
+      <c r="C20" s="22">
+        <v>45283</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="26"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="30"/>
+    <row r="21" spans="1:6" ht="248" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="21">
+        <v>2</v>
+      </c>
+      <c r="C21" s="22">
+        <v>45285</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="26"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="30"/>
+    <row r="22" spans="1:6" ht="225" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="21">
+        <v>2</v>
+      </c>
+      <c r="C22" s="22">
+        <v>45285</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="26"/>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="24"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="30"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="26"/>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="24"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="30"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="26"/>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="30"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="26"/>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="30"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="26"/>
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="24"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="30"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="26"/>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="24"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="30"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="26"/>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="22"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
     </row>
@@ -2394,7 +2444,7 @@
       </c>
       <c r="B30" s="11">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>